<commit_message>
updated timesheets for 11/9
</commit_message>
<xml_diff>
--- a/Admin/Ara Folder/Timesheet_10-25_10-31.xlsx
+++ b/Admin/Ara Folder/Timesheet_10-25_10-31.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Senior Design Project\Admin\Ara Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EA3776-2087-483E-ABEA-8DCEF33A762B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FF81D7-D8C3-4652-9B60-C3F663DB4A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,13 +746,19 @@
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>2</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="I7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="J7" s="7"/>
     </row>
@@ -764,12 +770,14 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
       <c r="I8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7"/>
     </row>
@@ -816,13 +824,15 @@
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9">
+        <v>0.5</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J11" s="7"/>
     </row>
@@ -912,15 +922,15 @@
       </c>
       <c r="E16" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="11">
         <f t="shared" si="1"/>
@@ -928,7 +938,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>7.25</v>
       </c>
       <c r="J16" s="12"/>
     </row>

</xml_diff>